<commit_message>
Changes of 20th June 2022
</commit_message>
<xml_diff>
--- a/RTE/src/main/resources/RTE Job Creation ForCrud.xlsx
+++ b/RTE/src/main/resources/RTE Job Creation ForCrud.xlsx
@@ -731,7 +731,7 @@
   <dimension ref="A1:CE3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="BP1" workbookViewId="0">
-      <selection activeCell="CB17" sqref="CB17"/>
+      <selection activeCell="CA2" sqref="CA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1039,7 +1039,7 @@
         <v>93</v>
       </c>
       <c r="P2" s="1">
-        <v>44691</v>
+        <v>44729</v>
       </c>
       <c r="Q2" s="1">
         <v>52993</v>
@@ -1048,10 +1048,10 @@
         <v>83</v>
       </c>
       <c r="S2" s="2">
-        <v>0</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="T2" s="2">
-        <v>0.96875</v>
+        <v>0.28125</v>
       </c>
       <c r="U2" t="s">
         <v>84</v>
@@ -1103,10 +1103,10 @@
         <v>87</v>
       </c>
       <c r="CA2" s="1">
-        <v>44691</v>
+        <v>44729</v>
       </c>
       <c r="CB2" s="2">
-        <v>3.472222222222222E-3</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="CC2">
         <v>0</v>

</xml_diff>